<commit_message>
update app test functionality to reflect no-display mode
</commit_message>
<xml_diff>
--- a/local/country_code_name.xlsx
+++ b/local/country_code_name.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81990" uniqueCount="23226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82462" uniqueCount="23698">
   <si>
     <t>ccode</t>
   </si>
@@ -68125,6 +68125,1422 @@
   </si>
   <si>
     <t>Saint Helena</t>
+  </si>
+  <si>
+    <t>Slovenia</t>
+  </si>
+  <si>
+    <t>Slovakia</t>
+  </si>
+  <si>
+    <t>Sierra Leone</t>
+  </si>
+  <si>
+    <t>San Marino</t>
+  </si>
+  <si>
+    <t>Senegal</t>
+  </si>
+  <si>
+    <t>Somalia</t>
+  </si>
+  <si>
+    <t>Suriname</t>
+  </si>
+  <si>
+    <t>South Sudan</t>
+  </si>
+  <si>
+    <t>Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t>El Salvador</t>
+  </si>
+  <si>
+    <t>Sint Maarten</t>
+  </si>
+  <si>
+    <t>Syrian Arab Republic</t>
+  </si>
+  <si>
+    <t>Eswatini</t>
+  </si>
+  <si>
+    <t>Turks and Caicos Islands</t>
+  </si>
+  <si>
+    <t>Chad</t>
+  </si>
+  <si>
+    <t>Togo</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Tajikistan</t>
+  </si>
+  <si>
+    <t>Tokelau</t>
+  </si>
+  <si>
+    <t>Timor-Leste</t>
+  </si>
+  <si>
+    <t>Turkmenistan</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Tonga</t>
+  </si>
+  <si>
+    <t>Turkey</t>
+  </si>
+  <si>
+    <t>Trinidad and Tobago</t>
+  </si>
+  <si>
+    <t>Tuvalu</t>
+  </si>
+  <si>
+    <t>United Republic of Tanzania</t>
+  </si>
+  <si>
+    <t>Ukraine</t>
+  </si>
+  <si>
+    <t>Uganda</t>
+  </si>
+  <si>
+    <t>United States of America</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Uzbekistan</t>
+  </si>
+  <si>
+    <t>Holy See</t>
+  </si>
+  <si>
+    <t>Saint Vincent and the Grenadines</t>
+  </si>
+  <si>
+    <t>Venezuela (Bolivarian Republic of)</t>
+  </si>
+  <si>
+    <t>British Virgin Islands</t>
+  </si>
+  <si>
+    <t>United States Virgin Islands</t>
+  </si>
+  <si>
+    <t>Viet Nam</t>
+  </si>
+  <si>
+    <t>Vanuatu</t>
+  </si>
+  <si>
+    <t>Wallis and Futuna</t>
+  </si>
+  <si>
+    <t>Samoa</t>
+  </si>
+  <si>
+    <t>Bonaire</t>
+  </si>
+  <si>
+    <t>Sint Eustatius</t>
+  </si>
+  <si>
+    <t>Saba</t>
+  </si>
+  <si>
+    <t>Kosovo[1]</t>
+  </si>
+  <si>
+    <t>Yemen</t>
+  </si>
+  <si>
+    <t>Mayotte</t>
+  </si>
+  <si>
+    <t>South Africa</t>
+  </si>
+  <si>
+    <t>Zambia</t>
+  </si>
+  <si>
+    <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>ccode</t>
+  </si>
+  <si>
+    <t>AD</t>
+  </si>
+  <si>
+    <t>AE</t>
+  </si>
+  <si>
+    <t>AF</t>
+  </si>
+  <si>
+    <t>AG</t>
+  </si>
+  <si>
+    <t>AI</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>AO</t>
+  </si>
+  <si>
+    <t>AR</t>
+  </si>
+  <si>
+    <t>AS</t>
+  </si>
+  <si>
+    <t>AT</t>
+  </si>
+  <si>
+    <t>AU</t>
+  </si>
+  <si>
+    <t>AW</t>
+  </si>
+  <si>
+    <t>AZ</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>BD</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>BF</t>
+  </si>
+  <si>
+    <t>BG</t>
+  </si>
+  <si>
+    <t>BH</t>
+  </si>
+  <si>
+    <t>BI</t>
+  </si>
+  <si>
+    <t>BJ</t>
+  </si>
+  <si>
+    <t>BL</t>
+  </si>
+  <si>
+    <t>BM</t>
+  </si>
+  <si>
+    <t>BN</t>
+  </si>
+  <si>
+    <t>BO</t>
+  </si>
+  <si>
+    <t>BR</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>BT</t>
+  </si>
+  <si>
+    <t>BW</t>
+  </si>
+  <si>
+    <t>BY</t>
+  </si>
+  <si>
+    <t>BZ</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>CD</t>
+  </si>
+  <si>
+    <t>CF</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>CI</t>
+  </si>
+  <si>
+    <t>CK</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>CM</t>
+  </si>
+  <si>
+    <t>CN</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>CV</t>
+  </si>
+  <si>
+    <t>CW</t>
+  </si>
+  <si>
+    <t>CY</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>DJ</t>
+  </si>
+  <si>
+    <t>DK</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>DZ</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>EE</t>
+  </si>
+  <si>
+    <t>EG</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>ES</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>FI</t>
+  </si>
+  <si>
+    <t>FJ</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>FO</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>GA</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>GD</t>
+  </si>
+  <si>
+    <t>GE</t>
+  </si>
+  <si>
+    <t>GF</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>GH</t>
+  </si>
+  <si>
+    <t>GI</t>
+  </si>
+  <si>
+    <t>GL</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>GN</t>
+  </si>
+  <si>
+    <t>GP</t>
+  </si>
+  <si>
+    <t>GQ</t>
+  </si>
+  <si>
+    <t>GR</t>
+  </si>
+  <si>
+    <t>GT</t>
+  </si>
+  <si>
+    <t>GU</t>
+  </si>
+  <si>
+    <t>GW</t>
+  </si>
+  <si>
+    <t>GY</t>
+  </si>
+  <si>
+    <t>HN</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>HT</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>IL</t>
+  </si>
+  <si>
+    <t>IM</t>
+  </si>
+  <si>
+    <t>IN</t>
+  </si>
+  <si>
+    <t>IQ</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>IS</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>JE</t>
+  </si>
+  <si>
+    <t>JM</t>
+  </si>
+  <si>
+    <t>JO</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
+    <t>KE</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KH</t>
+  </si>
+  <si>
+    <t>KI</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>KN</t>
+  </si>
+  <si>
+    <t>KP</t>
+  </si>
+  <si>
+    <t>KR</t>
+  </si>
+  <si>
+    <t>KW</t>
+  </si>
+  <si>
+    <t>KY</t>
+  </si>
+  <si>
+    <t>KZ</t>
+  </si>
+  <si>
+    <t>LA</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>LK</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>LS</t>
+  </si>
+  <si>
+    <t>LT</t>
+  </si>
+  <si>
+    <t>LU</t>
+  </si>
+  <si>
+    <t>LV</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>MD</t>
+  </si>
+  <si>
+    <t>ME</t>
+  </si>
+  <si>
+    <t>MF</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>MH</t>
+  </si>
+  <si>
+    <t>MK</t>
+  </si>
+  <si>
+    <t>ML</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>MN</t>
+  </si>
+  <si>
+    <t>MP</t>
+  </si>
+  <si>
+    <t>MQ</t>
+  </si>
+  <si>
+    <t>MR</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>MU</t>
+  </si>
+  <si>
+    <t>MV</t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>MX</t>
+  </si>
+  <si>
+    <t>MY</t>
+  </si>
+  <si>
+    <t>MZ</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NE</t>
+  </si>
+  <si>
+    <t>NG</t>
+  </si>
+  <si>
+    <t>NI</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>NP</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>NU</t>
+  </si>
+  <si>
+    <t>NZ</t>
+  </si>
+  <si>
+    <t>OM</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>PE</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>PH</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>PL</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>PW</t>
+  </si>
+  <si>
+    <t>PY</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>RE</t>
+  </si>
+  <si>
+    <t>RO</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>RU</t>
+  </si>
+  <si>
+    <t>RW</t>
+  </si>
+  <si>
+    <t>SA</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>SG</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t>SK</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>SO</t>
+  </si>
+  <si>
+    <t>SR</t>
+  </si>
+  <si>
+    <t>SS</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>SV</t>
+  </si>
+  <si>
+    <t>SX</t>
+  </si>
+  <si>
+    <t>SY</t>
+  </si>
+  <si>
+    <t>SZ</t>
+  </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>TD</t>
+  </si>
+  <si>
+    <t>TG</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>TJ</t>
+  </si>
+  <si>
+    <t>TK</t>
+  </si>
+  <si>
+    <t>TL</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>TN</t>
+  </si>
+  <si>
+    <t>TO</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>TT</t>
+  </si>
+  <si>
+    <t>TV</t>
+  </si>
+  <si>
+    <t>TZ</t>
+  </si>
+  <si>
+    <t>UA</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>UY</t>
+  </si>
+  <si>
+    <t>UZ</t>
+  </si>
+  <si>
+    <t>VA</t>
+  </si>
+  <si>
+    <t>VC</t>
+  </si>
+  <si>
+    <t>VE</t>
+  </si>
+  <si>
+    <t>VG</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>VN</t>
+  </si>
+  <si>
+    <t>VU</t>
+  </si>
+  <si>
+    <t>WF</t>
+  </si>
+  <si>
+    <t>WS</t>
+  </si>
+  <si>
+    <t>XA</t>
+  </si>
+  <si>
+    <t>XB</t>
+  </si>
+  <si>
+    <t>XC</t>
+  </si>
+  <si>
+    <t>XK</t>
+  </si>
+  <si>
+    <t>YE</t>
+  </si>
+  <si>
+    <t>YT</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>ZM</t>
+  </si>
+  <si>
+    <t>ZW</t>
+  </si>
+  <si>
+    <t>cname</t>
+  </si>
+  <si>
+    <t>Andorra</t>
+  </si>
+  <si>
+    <t>United Arab Emirates</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Antigua and Barbuda</t>
+  </si>
+  <si>
+    <t>Anguilla</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Armenia</t>
+  </si>
+  <si>
+    <t>Angola</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>American Samoa</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Aruba</t>
+  </si>
+  <si>
+    <t>Azerbaijan</t>
+  </si>
+  <si>
+    <t>Bosnia and Herzegovina</t>
+  </si>
+  <si>
+    <t>Barbados</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Burkina Faso</t>
+  </si>
+  <si>
+    <t>Bulgaria</t>
+  </si>
+  <si>
+    <t>Bahrain</t>
+  </si>
+  <si>
+    <t>Burundi</t>
+  </si>
+  <si>
+    <t>Benin</t>
+  </si>
+  <si>
+    <t>Saint Barthélemy</t>
+  </si>
+  <si>
+    <t>Bermuda</t>
+  </si>
+  <si>
+    <t>Brunei Darussalam</t>
+  </si>
+  <si>
+    <t>Bolivia (Plurinational State of)</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Bahamas</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Botswana</t>
+  </si>
+  <si>
+    <t>Belarus</t>
+  </si>
+  <si>
+    <t>Belize</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>Democratic Republic of the Congo</t>
+  </si>
+  <si>
+    <t>Central African Republic</t>
+  </si>
+  <si>
+    <t>Congo</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t>Côte d’Ivoire</t>
+  </si>
+  <si>
+    <t>Cook Islands</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>Cameroon</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Cuba</t>
+  </si>
+  <si>
+    <t>Cabo Verde</t>
+  </si>
+  <si>
+    <t>Curaçao</t>
+  </si>
+  <si>
+    <t>Cyprus</t>
+  </si>
+  <si>
+    <t>Czechia</t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Djibouti</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Dominica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>Estonia</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Finland</t>
+  </si>
+  <si>
+    <t>Fiji</t>
+  </si>
+  <si>
+    <t>Falkland Islands (Malvinas)</t>
+  </si>
+  <si>
+    <t>Micronesia (Federated States of)</t>
+  </si>
+  <si>
+    <t>Faroe Islands</t>
+  </si>
+  <si>
+    <t>France</t>
+  </si>
+  <si>
+    <t>Gabon</t>
+  </si>
+  <si>
+    <t>The United Kingdom</t>
+  </si>
+  <si>
+    <t>Grenada</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>French Guiana</t>
+  </si>
+  <si>
+    <t>Guernsey</t>
+  </si>
+  <si>
+    <t>Ghana</t>
+  </si>
+  <si>
+    <t>Gibraltar</t>
+  </si>
+  <si>
+    <t>Greenland</t>
+  </si>
+  <si>
+    <t>Gambia</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Guadeloupe</t>
+  </si>
+  <si>
+    <t>Equatorial Guinea</t>
+  </si>
+  <si>
+    <t>Greece</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t>Guinea-Bissau</t>
+  </si>
+  <si>
+    <t>Guyana</t>
+  </si>
+  <si>
+    <t>Honduras</t>
+  </si>
+  <si>
+    <t>Croatia</t>
+  </si>
+  <si>
+    <t>Haiti</t>
+  </si>
+  <si>
+    <t>Hungary</t>
+  </si>
+  <si>
+    <t>Indonesia</t>
+  </si>
+  <si>
+    <t>Ireland</t>
+  </si>
+  <si>
+    <t>Israel</t>
+  </si>
+  <si>
+    <t>Isle of Man</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Iraq</t>
+  </si>
+  <si>
+    <t>Iran (Islamic Republic of)</t>
+  </si>
+  <si>
+    <t>Iceland</t>
+  </si>
+  <si>
+    <t>Italy</t>
+  </si>
+  <si>
+    <t>Jersey</t>
+  </si>
+  <si>
+    <t>Jamaica</t>
+  </si>
+  <si>
+    <t>Jordan</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>Kenya</t>
+  </si>
+  <si>
+    <t>Kyrgyzstan</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Kiribati</t>
+  </si>
+  <si>
+    <t>Comoros</t>
+  </si>
+  <si>
+    <t>Saint Kitts and Nevis</t>
+  </si>
+  <si>
+    <t>Democratic People's Republic of Korea</t>
+  </si>
+  <si>
+    <t>Republic of Korea</t>
+  </si>
+  <si>
+    <t>Kuwait</t>
+  </si>
+  <si>
+    <t>Cayman Islands</t>
+  </si>
+  <si>
+    <t>Kazakhstan</t>
+  </si>
+  <si>
+    <t>Lao People's Democratic Republic</t>
+  </si>
+  <si>
+    <t>Lebanon</t>
+  </si>
+  <si>
+    <t>Saint Lucia</t>
+  </si>
+  <si>
+    <t>Liechtenstein</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Liberia</t>
+  </si>
+  <si>
+    <t>Lesotho</t>
+  </si>
+  <si>
+    <t>Lithuania</t>
+  </si>
+  <si>
+    <t>Luxembourg</t>
+  </si>
+  <si>
+    <t>Latvia</t>
+  </si>
+  <si>
+    <t>Libya</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>Republic of Moldova</t>
+  </si>
+  <si>
+    <t>Montenegro</t>
+  </si>
+  <si>
+    <t>Saint Martin</t>
+  </si>
+  <si>
+    <t>Madagascar</t>
+  </si>
+  <si>
+    <t>Marshall Islands</t>
+  </si>
+  <si>
+    <t>North Macedonia</t>
+  </si>
+  <si>
+    <t>Mali</t>
+  </si>
+  <si>
+    <t>Myanmar</t>
+  </si>
+  <si>
+    <t>Mongolia</t>
+  </si>
+  <si>
+    <t>Northern Mariana Islands (Commonwealth of the)</t>
+  </si>
+  <si>
+    <t>Martinique</t>
+  </si>
+  <si>
+    <t>Mauritania</t>
+  </si>
+  <si>
+    <t>Montserrat</t>
+  </si>
+  <si>
+    <t>Malta</t>
+  </si>
+  <si>
+    <t>Mauritius</t>
+  </si>
+  <si>
+    <t>Maldives</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Mozambique</t>
+  </si>
+  <si>
+    <t>Namibia</t>
+  </si>
+  <si>
+    <t>New Caledonia</t>
+  </si>
+  <si>
+    <t>Niger</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Nicaragua</t>
+  </si>
+  <si>
+    <t>Netherlands</t>
+  </si>
+  <si>
+    <t>Norway</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Nauru</t>
+  </si>
+  <si>
+    <t>Niue</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>Oman</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>French Polynesia</t>
+  </si>
+  <si>
+    <t>Papua New Guinea</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Poland</t>
+  </si>
+  <si>
+    <t>Saint Pierre and Miquelon</t>
+  </si>
+  <si>
+    <t>Pitcairn Islands</t>
+  </si>
+  <si>
+    <t>Puerto Rico</t>
+  </si>
+  <si>
+    <t>occupied Palestinian territory, including east Jerusalem</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Palau</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Qatar</t>
+  </si>
+  <si>
+    <t>Réunion</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Russian Federation</t>
+  </si>
+  <si>
+    <t>Rwanda</t>
+  </si>
+  <si>
+    <t>Saudi Arabia</t>
+  </si>
+  <si>
+    <t>Solomon Islands</t>
+  </si>
+  <si>
+    <t>Seychelles</t>
+  </si>
+  <si>
+    <t>Sudan</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Singapore</t>
   </si>
   <si>
     <t>Slovenia</t>
@@ -69711,7 +71127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="301">
+  <borders count="302">
     <border>
       <left/>
       <right/>
@@ -70019,11 +71435,12 @@
     <border/>
     <border/>
     <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="301">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -70325,6 +71742,7 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="298" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="299" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="300" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="301" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -70343,1890 +71761,1890 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="251" t="s">
-        <v>22754</v>
+        <v>23226</v>
       </c>
       <c r="B1" s="251" t="s">
-        <v>22990</v>
+        <v>23462</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="251" t="s">
-        <v>22755</v>
+        <v>23227</v>
       </c>
       <c r="B2" s="251" t="s">
-        <v>22991</v>
+        <v>23463</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="251" t="s">
-        <v>22756</v>
+        <v>23228</v>
       </c>
       <c r="B3" s="251" t="s">
-        <v>22992</v>
+        <v>23464</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="251" t="s">
-        <v>22757</v>
+        <v>23229</v>
       </c>
       <c r="B4" s="251" t="s">
-        <v>22993</v>
+        <v>23465</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="251" t="s">
-        <v>22758</v>
+        <v>23230</v>
       </c>
       <c r="B5" s="251" t="s">
-        <v>22994</v>
+        <v>23466</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="251" t="s">
-        <v>22759</v>
+        <v>23231</v>
       </c>
       <c r="B6" s="251" t="s">
-        <v>22995</v>
+        <v>23467</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="251" t="s">
-        <v>22760</v>
+        <v>23232</v>
       </c>
       <c r="B7" s="251" t="s">
-        <v>22996</v>
+        <v>23468</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="251" t="s">
-        <v>22761</v>
+        <v>23233</v>
       </c>
       <c r="B8" s="251" t="s">
-        <v>22997</v>
+        <v>23469</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="251" t="s">
-        <v>22762</v>
+        <v>23234</v>
       </c>
       <c r="B9" s="251" t="s">
-        <v>22998</v>
+        <v>23470</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="251" t="s">
-        <v>22763</v>
+        <v>23235</v>
       </c>
       <c r="B10" s="251" t="s">
-        <v>22999</v>
+        <v>23471</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="251" t="s">
-        <v>22764</v>
+        <v>23236</v>
       </c>
       <c r="B11" s="251" t="s">
-        <v>23000</v>
+        <v>23472</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="251" t="s">
-        <v>22765</v>
+        <v>23237</v>
       </c>
       <c r="B12" s="251" t="s">
-        <v>23001</v>
+        <v>23473</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="251" t="s">
-        <v>22766</v>
+        <v>23238</v>
       </c>
       <c r="B13" s="251" t="s">
-        <v>23002</v>
+        <v>23474</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="251" t="s">
-        <v>22767</v>
+        <v>23239</v>
       </c>
       <c r="B14" s="251" t="s">
-        <v>23003</v>
+        <v>23475</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="251" t="s">
-        <v>22768</v>
+        <v>23240</v>
       </c>
       <c r="B15" s="251" t="s">
-        <v>23004</v>
+        <v>23476</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="251" t="s">
-        <v>22769</v>
+        <v>23241</v>
       </c>
       <c r="B16" s="251" t="s">
-        <v>23005</v>
+        <v>23477</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="251" t="s">
-        <v>22770</v>
+        <v>23242</v>
       </c>
       <c r="B17" s="251" t="s">
-        <v>23006</v>
+        <v>23478</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="251" t="s">
-        <v>22771</v>
+        <v>23243</v>
       </c>
       <c r="B18" s="251" t="s">
-        <v>23007</v>
+        <v>23479</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="251" t="s">
-        <v>22772</v>
+        <v>23244</v>
       </c>
       <c r="B19" s="251" t="s">
-        <v>23008</v>
+        <v>23480</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="251" t="s">
-        <v>22773</v>
+        <v>23245</v>
       </c>
       <c r="B20" s="251" t="s">
-        <v>23009</v>
+        <v>23481</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="251" t="s">
-        <v>22774</v>
+        <v>23246</v>
       </c>
       <c r="B21" s="251" t="s">
-        <v>23010</v>
+        <v>23482</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="251" t="s">
-        <v>22775</v>
+        <v>23247</v>
       </c>
       <c r="B22" s="251" t="s">
-        <v>23011</v>
+        <v>23483</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="251" t="s">
-        <v>22776</v>
+        <v>23248</v>
       </c>
       <c r="B23" s="251" t="s">
-        <v>23012</v>
+        <v>23484</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="251" t="s">
-        <v>22777</v>
+        <v>23249</v>
       </c>
       <c r="B24" s="251" t="s">
-        <v>23013</v>
+        <v>23485</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="251" t="s">
-        <v>22778</v>
+        <v>23250</v>
       </c>
       <c r="B25" s="251" t="s">
-        <v>23014</v>
+        <v>23486</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="251" t="s">
-        <v>22779</v>
+        <v>23251</v>
       </c>
       <c r="B26" s="251" t="s">
-        <v>23015</v>
+        <v>23487</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="251" t="s">
-        <v>22780</v>
+        <v>23252</v>
       </c>
       <c r="B27" s="251" t="s">
-        <v>23016</v>
+        <v>23488</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="251" t="s">
-        <v>22781</v>
+        <v>23253</v>
       </c>
       <c r="B28" s="251" t="s">
-        <v>23017</v>
+        <v>23489</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="251" t="s">
-        <v>22782</v>
+        <v>23254</v>
       </c>
       <c r="B29" s="251" t="s">
-        <v>23018</v>
+        <v>23490</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="251" t="s">
-        <v>22783</v>
+        <v>23255</v>
       </c>
       <c r="B30" s="251" t="s">
-        <v>23019</v>
+        <v>23491</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="251" t="s">
-        <v>22784</v>
+        <v>23256</v>
       </c>
       <c r="B31" s="251" t="s">
-        <v>23020</v>
+        <v>23492</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="251" t="s">
-        <v>22785</v>
+        <v>23257</v>
       </c>
       <c r="B32" s="251" t="s">
-        <v>23021</v>
+        <v>23493</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="251" t="s">
-        <v>22786</v>
+        <v>23258</v>
       </c>
       <c r="B33" s="251" t="s">
-        <v>23022</v>
+        <v>23494</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="251" t="s">
-        <v>22787</v>
+        <v>23259</v>
       </c>
       <c r="B34" s="251" t="s">
-        <v>23023</v>
+        <v>23495</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="251" t="s">
-        <v>22788</v>
+        <v>23260</v>
       </c>
       <c r="B35" s="251" t="s">
-        <v>23024</v>
+        <v>23496</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="251" t="s">
-        <v>22789</v>
+        <v>23261</v>
       </c>
       <c r="B36" s="251" t="s">
-        <v>23025</v>
+        <v>23497</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="251" t="s">
-        <v>22790</v>
+        <v>23262</v>
       </c>
       <c r="B37" s="251" t="s">
-        <v>23026</v>
+        <v>23498</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="251" t="s">
-        <v>22791</v>
+        <v>23263</v>
       </c>
       <c r="B38" s="251" t="s">
-        <v>23027</v>
+        <v>23499</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="251" t="s">
-        <v>22792</v>
+        <v>23264</v>
       </c>
       <c r="B39" s="251" t="s">
-        <v>23028</v>
+        <v>23500</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="251" t="s">
-        <v>22793</v>
+        <v>23265</v>
       </c>
       <c r="B40" s="251" t="s">
-        <v>23029</v>
+        <v>23501</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="251" t="s">
-        <v>22794</v>
+        <v>23266</v>
       </c>
       <c r="B41" s="251" t="s">
-        <v>23030</v>
+        <v>23502</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="251" t="s">
-        <v>22795</v>
+        <v>23267</v>
       </c>
       <c r="B42" s="251" t="s">
-        <v>23031</v>
+        <v>23503</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="251" t="s">
-        <v>22796</v>
+        <v>23268</v>
       </c>
       <c r="B43" s="251" t="s">
-        <v>23032</v>
+        <v>23504</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="251" t="s">
-        <v>22797</v>
+        <v>23269</v>
       </c>
       <c r="B44" s="251" t="s">
-        <v>23033</v>
+        <v>23505</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="251" t="s">
-        <v>22798</v>
+        <v>23270</v>
       </c>
       <c r="B45" s="251" t="s">
-        <v>23034</v>
+        <v>23506</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="251" t="s">
-        <v>22799</v>
+        <v>23271</v>
       </c>
       <c r="B46" s="251" t="s">
-        <v>23035</v>
+        <v>23507</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="251" t="s">
-        <v>22800</v>
+        <v>23272</v>
       </c>
       <c r="B47" s="251" t="s">
-        <v>23036</v>
+        <v>23508</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="251" t="s">
-        <v>22801</v>
+        <v>23273</v>
       </c>
       <c r="B48" s="251" t="s">
-        <v>23037</v>
+        <v>23509</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="251" t="s">
-        <v>22802</v>
+        <v>23274</v>
       </c>
       <c r="B49" s="251" t="s">
-        <v>23038</v>
+        <v>23510</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="251" t="s">
-        <v>22803</v>
+        <v>23275</v>
       </c>
       <c r="B50" s="251" t="s">
-        <v>23039</v>
+        <v>23511</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="251" t="s">
-        <v>22804</v>
+        <v>23276</v>
       </c>
       <c r="B51" s="251" t="s">
-        <v>23040</v>
+        <v>23512</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="251" t="s">
-        <v>22805</v>
+        <v>23277</v>
       </c>
       <c r="B52" s="251" t="s">
-        <v>23041</v>
+        <v>23513</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="251" t="s">
-        <v>22806</v>
+        <v>23278</v>
       </c>
       <c r="B53" s="251" t="s">
-        <v>23042</v>
+        <v>23514</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="251" t="s">
-        <v>22807</v>
+        <v>23279</v>
       </c>
       <c r="B54" s="251" t="s">
-        <v>23043</v>
+        <v>23515</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="251" t="s">
-        <v>22808</v>
+        <v>23280</v>
       </c>
       <c r="B55" s="251" t="s">
-        <v>23044</v>
+        <v>23516</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="251" t="s">
-        <v>22809</v>
+        <v>23281</v>
       </c>
       <c r="B56" s="251" t="s">
-        <v>23045</v>
+        <v>23517</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="251" t="s">
-        <v>22810</v>
+        <v>23282</v>
       </c>
       <c r="B57" s="251" t="s">
-        <v>23046</v>
+        <v>23518</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="251" t="s">
-        <v>22811</v>
+        <v>23283</v>
       </c>
       <c r="B58" s="251" t="s">
-        <v>23047</v>
+        <v>23519</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="251" t="s">
-        <v>22812</v>
+        <v>23284</v>
       </c>
       <c r="B59" s="251" t="s">
-        <v>23048</v>
+        <v>23520</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="251" t="s">
-        <v>22813</v>
+        <v>23285</v>
       </c>
       <c r="B60" s="251" t="s">
-        <v>23049</v>
+        <v>23521</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="251" t="s">
-        <v>22814</v>
+        <v>23286</v>
       </c>
       <c r="B61" s="251" t="s">
-        <v>23050</v>
+        <v>23522</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="251" t="s">
-        <v>22815</v>
+        <v>23287</v>
       </c>
       <c r="B62" s="251" t="s">
-        <v>23051</v>
+        <v>23523</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="251" t="s">
-        <v>22816</v>
+        <v>23288</v>
       </c>
       <c r="B63" s="251" t="s">
-        <v>23052</v>
+        <v>23524</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="251" t="s">
-        <v>22817</v>
+        <v>23289</v>
       </c>
       <c r="B64" s="251" t="s">
-        <v>23053</v>
+        <v>23525</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="251" t="s">
-        <v>22818</v>
+        <v>23290</v>
       </c>
       <c r="B65" s="251" t="s">
-        <v>23054</v>
+        <v>23526</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="251" t="s">
-        <v>22819</v>
+        <v>23291</v>
       </c>
       <c r="B66" s="251" t="s">
-        <v>23055</v>
+        <v>23527</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="251" t="s">
-        <v>22820</v>
+        <v>23292</v>
       </c>
       <c r="B67" s="251" t="s">
-        <v>23056</v>
+        <v>23528</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="251" t="s">
-        <v>22821</v>
+        <v>23293</v>
       </c>
       <c r="B68" s="251" t="s">
-        <v>23057</v>
+        <v>23529</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="251" t="s">
-        <v>22822</v>
+        <v>23294</v>
       </c>
       <c r="B69" s="251" t="s">
-        <v>23058</v>
+        <v>23530</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="251" t="s">
-        <v>22823</v>
+        <v>23295</v>
       </c>
       <c r="B70" s="251" t="s">
-        <v>23059</v>
+        <v>23531</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="251" t="s">
-        <v>22824</v>
+        <v>23296</v>
       </c>
       <c r="B71" s="251" t="s">
-        <v>23060</v>
+        <v>23532</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="251" t="s">
-        <v>22825</v>
+        <v>23297</v>
       </c>
       <c r="B72" s="251" t="s">
-        <v>23061</v>
+        <v>23533</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="251" t="s">
-        <v>22826</v>
+        <v>23298</v>
       </c>
       <c r="B73" s="251" t="s">
-        <v>23062</v>
+        <v>23534</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="251" t="s">
-        <v>22827</v>
+        <v>23299</v>
       </c>
       <c r="B74" s="251" t="s">
-        <v>23063</v>
+        <v>23535</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="251" t="s">
-        <v>22828</v>
+        <v>23300</v>
       </c>
       <c r="B75" s="251" t="s">
-        <v>23064</v>
+        <v>23536</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="251" t="s">
-        <v>22829</v>
+        <v>23301</v>
       </c>
       <c r="B76" s="251" t="s">
-        <v>23065</v>
+        <v>23537</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="251" t="s">
-        <v>22830</v>
+        <v>23302</v>
       </c>
       <c r="B77" s="251" t="s">
-        <v>23066</v>
+        <v>23538</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="251" t="s">
-        <v>22831</v>
+        <v>23303</v>
       </c>
       <c r="B78" s="251" t="s">
-        <v>23067</v>
+        <v>23539</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="251" t="s">
-        <v>22832</v>
+        <v>23304</v>
       </c>
       <c r="B79" s="251" t="s">
-        <v>23068</v>
+        <v>23540</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="251" t="s">
-        <v>22833</v>
+        <v>23305</v>
       </c>
       <c r="B80" s="251" t="s">
-        <v>23069</v>
+        <v>23541</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="251" t="s">
-        <v>22834</v>
+        <v>23306</v>
       </c>
       <c r="B81" s="251" t="s">
-        <v>23070</v>
+        <v>23542</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" s="251" t="s">
-        <v>22835</v>
+        <v>23307</v>
       </c>
       <c r="B82" s="251" t="s">
-        <v>23071</v>
+        <v>23543</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" s="251" t="s">
-        <v>22836</v>
+        <v>23308</v>
       </c>
       <c r="B83" s="251" t="s">
-        <v>23072</v>
+        <v>23544</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="251" t="s">
-        <v>22837</v>
+        <v>23309</v>
       </c>
       <c r="B84" s="251" t="s">
-        <v>23073</v>
+        <v>23545</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="251" t="s">
-        <v>22838</v>
+        <v>23310</v>
       </c>
       <c r="B85" s="251" t="s">
-        <v>23074</v>
+        <v>23546</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="251" t="s">
-        <v>22839</v>
+        <v>23311</v>
       </c>
       <c r="B86" s="251" t="s">
-        <v>23075</v>
+        <v>23547</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="251" t="s">
-        <v>22840</v>
+        <v>23312</v>
       </c>
       <c r="B87" s="251" t="s">
-        <v>23076</v>
+        <v>23548</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="251" t="s">
-        <v>22841</v>
+        <v>23313</v>
       </c>
       <c r="B88" s="251" t="s">
-        <v>23077</v>
+        <v>23549</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="251" t="s">
-        <v>22842</v>
+        <v>23314</v>
       </c>
       <c r="B89" s="251" t="s">
-        <v>23078</v>
+        <v>23550</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="251" t="s">
-        <v>22843</v>
+        <v>23315</v>
       </c>
       <c r="B90" s="251" t="s">
-        <v>23079</v>
+        <v>23551</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="251" t="s">
-        <v>22844</v>
+        <v>23316</v>
       </c>
       <c r="B91" s="251" t="s">
-        <v>23080</v>
+        <v>23552</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="251" t="s">
-        <v>22845</v>
+        <v>23317</v>
       </c>
       <c r="B92" s="251" t="s">
-        <v>23081</v>
+        <v>23553</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="251" t="s">
-        <v>22846</v>
+        <v>23318</v>
       </c>
       <c r="B93" s="251" t="s">
-        <v>23082</v>
+        <v>23554</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="251" t="s">
-        <v>22847</v>
+        <v>23319</v>
       </c>
       <c r="B94" s="251" t="s">
-        <v>23083</v>
+        <v>23555</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="251" t="s">
-        <v>22848</v>
+        <v>23320</v>
       </c>
       <c r="B95" s="251" t="s">
-        <v>23084</v>
+        <v>23556</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="251" t="s">
-        <v>22849</v>
+        <v>23321</v>
       </c>
       <c r="B96" s="251" t="s">
-        <v>23085</v>
+        <v>23557</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="251" t="s">
-        <v>22850</v>
+        <v>23322</v>
       </c>
       <c r="B97" s="251" t="s">
-        <v>23086</v>
+        <v>23558</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="251" t="s">
-        <v>22851</v>
+        <v>23323</v>
       </c>
       <c r="B98" s="251" t="s">
-        <v>23087</v>
+        <v>23559</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="251" t="s">
-        <v>22852</v>
+        <v>23324</v>
       </c>
       <c r="B99" s="251" t="s">
-        <v>23088</v>
+        <v>23560</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="251" t="s">
-        <v>22853</v>
+        <v>23325</v>
       </c>
       <c r="B100" s="251" t="s">
-        <v>23089</v>
+        <v>23561</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="251" t="s">
-        <v>22854</v>
+        <v>23326</v>
       </c>
       <c r="B101" s="251" t="s">
-        <v>23090</v>
+        <v>23562</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="251" t="s">
-        <v>22855</v>
+        <v>23327</v>
       </c>
       <c r="B102" s="251" t="s">
-        <v>23091</v>
+        <v>23563</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="251" t="s">
-        <v>22856</v>
+        <v>23328</v>
       </c>
       <c r="B103" s="251" t="s">
-        <v>23092</v>
+        <v>23564</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="251" t="s">
-        <v>22857</v>
+        <v>23329</v>
       </c>
       <c r="B104" s="251" t="s">
-        <v>23093</v>
+        <v>23565</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="251" t="s">
-        <v>22858</v>
+        <v>23330</v>
       </c>
       <c r="B105" s="251" t="s">
-        <v>23094</v>
+        <v>23566</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="251" t="s">
-        <v>22859</v>
+        <v>23331</v>
       </c>
       <c r="B106" s="251" t="s">
-        <v>23095</v>
+        <v>23567</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="251" t="s">
-        <v>22860</v>
+        <v>23332</v>
       </c>
       <c r="B107" s="251" t="s">
-        <v>23096</v>
+        <v>23568</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="251" t="s">
-        <v>22861</v>
+        <v>23333</v>
       </c>
       <c r="B108" s="251" t="s">
-        <v>23097</v>
+        <v>23569</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="251" t="s">
-        <v>22862</v>
+        <v>23334</v>
       </c>
       <c r="B109" s="251" t="s">
-        <v>23098</v>
+        <v>23570</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="251" t="s">
-        <v>22863</v>
+        <v>23335</v>
       </c>
       <c r="B110" s="251" t="s">
-        <v>23099</v>
+        <v>23571</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="251" t="s">
-        <v>22864</v>
+        <v>23336</v>
       </c>
       <c r="B111" s="251" t="s">
-        <v>23100</v>
+        <v>23572</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="251" t="s">
-        <v>22865</v>
+        <v>23337</v>
       </c>
       <c r="B112" s="251" t="s">
-        <v>23101</v>
+        <v>23573</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="251" t="s">
-        <v>22866</v>
+        <v>23338</v>
       </c>
       <c r="B113" s="251" t="s">
-        <v>23102</v>
+        <v>23574</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="251" t="s">
-        <v>22867</v>
+        <v>23339</v>
       </c>
       <c r="B114" s="251" t="s">
-        <v>23103</v>
+        <v>23575</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="251" t="s">
-        <v>22868</v>
+        <v>23340</v>
       </c>
       <c r="B115" s="251" t="s">
-        <v>23104</v>
+        <v>23576</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="251" t="s">
-        <v>22869</v>
+        <v>23341</v>
       </c>
       <c r="B116" s="251" t="s">
-        <v>23105</v>
+        <v>23577</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="251" t="s">
-        <v>22870</v>
+        <v>23342</v>
       </c>
       <c r="B117" s="251" t="s">
-        <v>23106</v>
+        <v>23578</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="251" t="s">
-        <v>22871</v>
+        <v>23343</v>
       </c>
       <c r="B118" s="251" t="s">
-        <v>23107</v>
+        <v>23579</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="251" t="s">
-        <v>22872</v>
+        <v>23344</v>
       </c>
       <c r="B119" s="251" t="s">
-        <v>23108</v>
+        <v>23580</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="251" t="s">
-        <v>22873</v>
+        <v>23345</v>
       </c>
       <c r="B120" s="251" t="s">
-        <v>23109</v>
+        <v>23581</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="251" t="s">
-        <v>22874</v>
+        <v>23346</v>
       </c>
       <c r="B121" s="251" t="s">
-        <v>23110</v>
+        <v>23582</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" s="251" t="s">
-        <v>22875</v>
+        <v>23347</v>
       </c>
       <c r="B122" s="251" t="s">
-        <v>23111</v>
+        <v>23583</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" s="251" t="s">
-        <v>22876</v>
+        <v>23348</v>
       </c>
       <c r="B123" s="251" t="s">
-        <v>23112</v>
+        <v>23584</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" s="251" t="s">
-        <v>22877</v>
+        <v>23349</v>
       </c>
       <c r="B124" s="251" t="s">
-        <v>23113</v>
+        <v>23585</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" s="251" t="s">
-        <v>22878</v>
+        <v>23350</v>
       </c>
       <c r="B125" s="251" t="s">
-        <v>23114</v>
+        <v>23586</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" s="251" t="s">
-        <v>22879</v>
+        <v>23351</v>
       </c>
       <c r="B126" s="251" t="s">
-        <v>23115</v>
+        <v>23587</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="251" t="s">
-        <v>22880</v>
+        <v>23352</v>
       </c>
       <c r="B127" s="251" t="s">
-        <v>23116</v>
+        <v>23588</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" s="251" t="s">
-        <v>22881</v>
+        <v>23353</v>
       </c>
       <c r="B128" s="251" t="s">
-        <v>23117</v>
+        <v>23589</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" s="251" t="s">
-        <v>22882</v>
+        <v>23354</v>
       </c>
       <c r="B129" s="251" t="s">
-        <v>23118</v>
+        <v>23590</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" s="251" t="s">
-        <v>22883</v>
+        <v>23355</v>
       </c>
       <c r="B130" s="251" t="s">
-        <v>23119</v>
+        <v>23591</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" s="251" t="s">
-        <v>22884</v>
+        <v>23356</v>
       </c>
       <c r="B131" s="251" t="s">
-        <v>23120</v>
+        <v>23592</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" s="251" t="s">
-        <v>22885</v>
+        <v>23357</v>
       </c>
       <c r="B132" s="251" t="s">
-        <v>23121</v>
+        <v>23593</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="251" t="s">
-        <v>22886</v>
+        <v>23358</v>
       </c>
       <c r="B133" s="251" t="s">
-        <v>23122</v>
+        <v>23594</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" s="251" t="s">
-        <v>22887</v>
+        <v>23359</v>
       </c>
       <c r="B134" s="251" t="s">
-        <v>23123</v>
+        <v>23595</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" s="251" t="s">
-        <v>22888</v>
+        <v>23360</v>
       </c>
       <c r="B135" s="251" t="s">
-        <v>23124</v>
+        <v>23596</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" s="251" t="s">
-        <v>22889</v>
+        <v>23361</v>
       </c>
       <c r="B136" s="251" t="s">
-        <v>23125</v>
+        <v>23597</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" s="251" t="s">
-        <v>22890</v>
+        <v>23362</v>
       </c>
       <c r="B137" s="251" t="s">
-        <v>23126</v>
+        <v>23598</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="251" t="s">
-        <v>22891</v>
+        <v>23363</v>
       </c>
       <c r="B138" s="251" t="s">
-        <v>23127</v>
+        <v>23599</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" s="251" t="s">
-        <v>22892</v>
+        <v>23364</v>
       </c>
       <c r="B139" s="251" t="s">
-        <v>23128</v>
+        <v>23600</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" s="251" t="s">
-        <v>22893</v>
+        <v>23365</v>
       </c>
       <c r="B140" s="251" t="s">
-        <v>23129</v>
+        <v>23601</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" s="251" t="s">
-        <v>22894</v>
+        <v>23366</v>
       </c>
       <c r="B141" s="251" t="s">
-        <v>23130</v>
+        <v>23602</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" s="251" t="s">
-        <v>22895</v>
+        <v>23367</v>
       </c>
       <c r="B142" s="251" t="s">
-        <v>23131</v>
+        <v>23603</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" s="251" t="s">
-        <v>22896</v>
+        <v>23368</v>
       </c>
       <c r="B143" s="251" t="s">
-        <v>23132</v>
+        <v>23604</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" s="251" t="s">
-        <v>22897</v>
+        <v>23369</v>
       </c>
       <c r="B144" s="251" t="s">
-        <v>23133</v>
+        <v>23605</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" s="251" t="s">
-        <v>22898</v>
+        <v>23370</v>
       </c>
       <c r="B145" s="251" t="s">
-        <v>23134</v>
+        <v>23606</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" s="251" t="s">
-        <v>22899</v>
+        <v>23371</v>
       </c>
       <c r="B146" s="251" t="s">
-        <v>23135</v>
+        <v>23607</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" s="251" t="s">
-        <v>22900</v>
+        <v>23372</v>
       </c>
       <c r="B147" s="251" t="s">
-        <v>23136</v>
+        <v>23608</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" s="251" t="s">
-        <v>22901</v>
+        <v>23373</v>
       </c>
       <c r="B148" s="251" t="s">
-        <v>23137</v>
+        <v>23609</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" s="251" t="s">
-        <v>22902</v>
+        <v>23374</v>
       </c>
       <c r="B149" s="251" t="s">
-        <v>23138</v>
+        <v>23610</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" s="251" t="s">
-        <v>22903</v>
+        <v>23375</v>
       </c>
       <c r="B150" s="251" t="s">
-        <v>23139</v>
+        <v>23611</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" s="251" t="s">
-        <v>22904</v>
+        <v>23376</v>
       </c>
       <c r="B151" s="251" t="s">
-        <v>23140</v>
+        <v>23612</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" s="251" t="s">
-        <v>22905</v>
+        <v>23377</v>
       </c>
       <c r="B152" s="251" t="s">
-        <v>23141</v>
+        <v>23613</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" s="251" t="s">
-        <v>22906</v>
+        <v>23378</v>
       </c>
       <c r="B153" s="251" t="s">
-        <v>23142</v>
+        <v>23614</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" s="251" t="s">
-        <v>22907</v>
+        <v>23379</v>
       </c>
       <c r="B154" s="251" t="s">
-        <v>23143</v>
+        <v>23615</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" s="251" t="s">
-        <v>22908</v>
+        <v>23380</v>
       </c>
       <c r="B155" s="251" t="s">
-        <v>23144</v>
+        <v>23616</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" s="251" t="s">
-        <v>22909</v>
+        <v>23381</v>
       </c>
       <c r="B156" s="251" t="s">
-        <v>23145</v>
+        <v>23617</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" s="251" t="s">
-        <v>22910</v>
+        <v>23382</v>
       </c>
       <c r="B157" s="251" t="s">
-        <v>23146</v>
+        <v>23618</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="251" t="s">
-        <v>22911</v>
+        <v>23383</v>
       </c>
       <c r="B158" s="251" t="s">
-        <v>23147</v>
+        <v>23619</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" s="251" t="s">
-        <v>22912</v>
+        <v>23384</v>
       </c>
       <c r="B159" s="251" t="s">
-        <v>23148</v>
+        <v>23620</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" s="251" t="s">
-        <v>22913</v>
+        <v>23385</v>
       </c>
       <c r="B160" s="251" t="s">
-        <v>23149</v>
+        <v>23621</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" s="251" t="s">
-        <v>22914</v>
+        <v>23386</v>
       </c>
       <c r="B161" s="251" t="s">
-        <v>23150</v>
+        <v>23622</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" s="251" t="s">
-        <v>22915</v>
+        <v>23387</v>
       </c>
       <c r="B162" s="251" t="s">
-        <v>23151</v>
+        <v>23623</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" s="251" t="s">
-        <v>22916</v>
+        <v>23388</v>
       </c>
       <c r="B163" s="251" t="s">
-        <v>23152</v>
+        <v>23624</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" s="251" t="s">
-        <v>22917</v>
+        <v>23389</v>
       </c>
       <c r="B164" s="251" t="s">
-        <v>23153</v>
+        <v>23625</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="251" t="s">
-        <v>22918</v>
+        <v>23390</v>
       </c>
       <c r="B165" s="251" t="s">
-        <v>23154</v>
+        <v>23626</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" s="251" t="s">
-        <v>22919</v>
+        <v>23391</v>
       </c>
       <c r="B166" s="251" t="s">
-        <v>23155</v>
+        <v>23627</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" s="251" t="s">
-        <v>22920</v>
+        <v>23392</v>
       </c>
       <c r="B167" s="251" t="s">
-        <v>23156</v>
+        <v>23628</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" s="251" t="s">
-        <v>22921</v>
+        <v>23393</v>
       </c>
       <c r="B168" s="251" t="s">
-        <v>23157</v>
+        <v>23629</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" s="251" t="s">
-        <v>22922</v>
+        <v>23394</v>
       </c>
       <c r="B169" s="251" t="s">
-        <v>23158</v>
+        <v>23630</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" s="251" t="s">
-        <v>22923</v>
+        <v>23395</v>
       </c>
       <c r="B170" s="251" t="s">
-        <v>23159</v>
+        <v>23631</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" s="251" t="s">
-        <v>22924</v>
+        <v>23396</v>
       </c>
       <c r="B171" s="251" t="s">
-        <v>23160</v>
+        <v>23632</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" s="251" t="s">
-        <v>22925</v>
+        <v>23397</v>
       </c>
       <c r="B172" s="251" t="s">
-        <v>23161</v>
+        <v>23633</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" s="251" t="s">
-        <v>22926</v>
+        <v>23398</v>
       </c>
       <c r="B173" s="251" t="s">
-        <v>23162</v>
+        <v>23634</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" s="251" t="s">
-        <v>22927</v>
+        <v>23399</v>
       </c>
       <c r="B174" s="251" t="s">
-        <v>23163</v>
+        <v>23635</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" s="251" t="s">
-        <v>22928</v>
+        <v>23400</v>
       </c>
       <c r="B175" s="251" t="s">
-        <v>23164</v>
+        <v>23636</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" s="251" t="s">
-        <v>22929</v>
+        <v>23401</v>
       </c>
       <c r="B176" s="251" t="s">
-        <v>23165</v>
+        <v>23637</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" s="251" t="s">
-        <v>22930</v>
+        <v>23402</v>
       </c>
       <c r="B177" s="251" t="s">
-        <v>23166</v>
+        <v>23638</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" s="251" t="s">
-        <v>22931</v>
+        <v>23403</v>
       </c>
       <c r="B178" s="251" t="s">
-        <v>23167</v>
+        <v>23639</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" s="251" t="s">
-        <v>22932</v>
+        <v>23404</v>
       </c>
       <c r="B179" s="251" t="s">
-        <v>23168</v>
+        <v>23640</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" s="251" t="s">
-        <v>22933</v>
+        <v>23405</v>
       </c>
       <c r="B180" s="251" t="s">
-        <v>23169</v>
+        <v>23641</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="251" t="s">
-        <v>22934</v>
+        <v>23406</v>
       </c>
       <c r="B181" s="251" t="s">
-        <v>23170</v>
+        <v>23642</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" s="251" t="s">
-        <v>22935</v>
+        <v>23407</v>
       </c>
       <c r="B182" s="251" t="s">
-        <v>23171</v>
+        <v>23643</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" s="251" t="s">
-        <v>22936</v>
+        <v>23408</v>
       </c>
       <c r="B183" s="251" t="s">
-        <v>23172</v>
+        <v>23644</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" s="251" t="s">
-        <v>22937</v>
+        <v>23409</v>
       </c>
       <c r="B184" s="251" t="s">
-        <v>23173</v>
+        <v>23645</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" s="251" t="s">
-        <v>22938</v>
+        <v>23410</v>
       </c>
       <c r="B185" s="251" t="s">
-        <v>23174</v>
+        <v>23646</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" s="251" t="s">
-        <v>22939</v>
+        <v>23411</v>
       </c>
       <c r="B186" s="251" t="s">
-        <v>23175</v>
+        <v>23647</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" s="251" t="s">
-        <v>22940</v>
+        <v>23412</v>
       </c>
       <c r="B187" s="251" t="s">
-        <v>23176</v>
+        <v>23648</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" s="251" t="s">
-        <v>22941</v>
+        <v>23413</v>
       </c>
       <c r="B188" s="251" t="s">
-        <v>23177</v>
+        <v>23649</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" s="251" t="s">
-        <v>22942</v>
+        <v>23414</v>
       </c>
       <c r="B189" s="251" t="s">
-        <v>23178</v>
+        <v>23650</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" s="251" t="s">
-        <v>22943</v>
+        <v>23415</v>
       </c>
       <c r="B190" s="251" t="s">
-        <v>23179</v>
+        <v>23651</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" s="251" t="s">
-        <v>22944</v>
+        <v>23416</v>
       </c>
       <c r="B191" s="251" t="s">
-        <v>23180</v>
+        <v>23652</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="251" t="s">
-        <v>22945</v>
+        <v>23417</v>
       </c>
       <c r="B192" s="251" t="s">
-        <v>23181</v>
+        <v>23653</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" s="251" t="s">
-        <v>22946</v>
+        <v>23418</v>
       </c>
       <c r="B193" s="251" t="s">
-        <v>23182</v>
+        <v>23654</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" s="251" t="s">
-        <v>22947</v>
+        <v>23419</v>
       </c>
       <c r="B194" s="251" t="s">
-        <v>23183</v>
+        <v>23655</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" s="251" t="s">
-        <v>22948</v>
+        <v>23420</v>
       </c>
       <c r="B195" s="251" t="s">
-        <v>23184</v>
+        <v>23656</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" s="251" t="s">
-        <v>22949</v>
+        <v>23421</v>
       </c>
       <c r="B196" s="251" t="s">
-        <v>23185</v>
+        <v>23657</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" s="251" t="s">
-        <v>22950</v>
+        <v>23422</v>
       </c>
       <c r="B197" s="251" t="s">
-        <v>23186</v>
+        <v>23658</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" s="251" t="s">
-        <v>22951</v>
+        <v>23423</v>
       </c>
       <c r="B198" s="251" t="s">
-        <v>23187</v>
+        <v>23659</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" s="251" t="s">
-        <v>22952</v>
+        <v>23424</v>
       </c>
       <c r="B199" s="251" t="s">
-        <v>23188</v>
+        <v>23660</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" s="251" t="s">
-        <v>22953</v>
+        <v>23425</v>
       </c>
       <c r="B200" s="251" t="s">
-        <v>23189</v>
+        <v>23661</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" s="251" t="s">
-        <v>22954</v>
+        <v>23426</v>
       </c>
       <c r="B201" s="251" t="s">
-        <v>23190</v>
+        <v>23662</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" s="251" t="s">
-        <v>22955</v>
+        <v>23427</v>
       </c>
       <c r="B202" s="251" t="s">
-        <v>23191</v>
+        <v>23663</v>
       </c>
     </row>
     <row r="203">
       <c r="A203" s="251" t="s">
-        <v>22956</v>
+        <v>23428</v>
       </c>
       <c r="B203" s="251" t="s">
-        <v>23192</v>
+        <v>23664</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" s="251" t="s">
-        <v>22957</v>
+        <v>23429</v>
       </c>
       <c r="B204" s="251" t="s">
-        <v>23193</v>
+        <v>23665</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" s="251" t="s">
-        <v>22958</v>
+        <v>23430</v>
       </c>
       <c r="B205" s="251" t="s">
-        <v>23194</v>
+        <v>23666</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" s="251" t="s">
-        <v>22959</v>
+        <v>23431</v>
       </c>
       <c r="B206" s="251" t="s">
-        <v>23195</v>
+        <v>23667</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" s="251" t="s">
-        <v>22960</v>
+        <v>23432</v>
       </c>
       <c r="B207" s="251" t="s">
-        <v>23196</v>
+        <v>23668</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" s="251" t="s">
-        <v>22961</v>
+        <v>23433</v>
       </c>
       <c r="B208" s="251" t="s">
-        <v>23197</v>
+        <v>23669</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" s="251" t="s">
-        <v>22962</v>
+        <v>23434</v>
       </c>
       <c r="B209" s="251" t="s">
-        <v>23198</v>
+        <v>23670</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" s="251" t="s">
-        <v>22963</v>
+        <v>23435</v>
       </c>
       <c r="B210" s="251" t="s">
-        <v>23199</v>
+        <v>23671</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" s="251" t="s">
-        <v>22964</v>
+        <v>23436</v>
       </c>
       <c r="B211" s="251" t="s">
-        <v>23200</v>
+        <v>23672</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" s="251" t="s">
-        <v>22965</v>
+        <v>23437</v>
       </c>
       <c r="B212" s="251" t="s">
-        <v>23201</v>
+        <v>23673</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" s="251" t="s">
-        <v>22966</v>
+        <v>23438</v>
       </c>
       <c r="B213" s="251" t="s">
-        <v>23202</v>
+        <v>23674</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" s="251" t="s">
-        <v>22967</v>
+        <v>23439</v>
       </c>
       <c r="B214" s="251" t="s">
-        <v>23203</v>
+        <v>23675</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" s="251" t="s">
-        <v>22968</v>
+        <v>23440</v>
       </c>
       <c r="B215" s="251" t="s">
-        <v>23204</v>
+        <v>23676</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" s="251" t="s">
-        <v>22969</v>
+        <v>23441</v>
       </c>
       <c r="B216" s="251" t="s">
-        <v>23205</v>
+        <v>23677</v>
       </c>
     </row>
     <row r="217">
       <c r="A217" s="251" t="s">
-        <v>22970</v>
+        <v>23442</v>
       </c>
       <c r="B217" s="251" t="s">
-        <v>23206</v>
+        <v>23678</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" s="251" t="s">
-        <v>22971</v>
+        <v>23443</v>
       </c>
       <c r="B218" s="251" t="s">
-        <v>23207</v>
+        <v>23679</v>
       </c>
     </row>
     <row r="219">
       <c r="A219" s="251" t="s">
-        <v>22972</v>
+        <v>23444</v>
       </c>
       <c r="B219" s="251" t="s">
-        <v>23208</v>
+        <v>23680</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" s="251" t="s">
-        <v>22973</v>
+        <v>23445</v>
       </c>
       <c r="B220" s="251" t="s">
-        <v>23209</v>
+        <v>23681</v>
       </c>
     </row>
     <row r="221">
       <c r="A221" s="251" t="s">
-        <v>22974</v>
+        <v>23446</v>
       </c>
       <c r="B221" s="251" t="s">
-        <v>23210</v>
+        <v>23682</v>
       </c>
     </row>
     <row r="222">
       <c r="A222" s="251" t="s">
-        <v>22975</v>
+        <v>23447</v>
       </c>
       <c r="B222" s="251" t="s">
-        <v>23211</v>
+        <v>23683</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" s="251" t="s">
-        <v>22976</v>
+        <v>23448</v>
       </c>
       <c r="B223" s="251" t="s">
-        <v>23212</v>
+        <v>23684</v>
       </c>
     </row>
     <row r="224">
       <c r="A224" s="251" t="s">
-        <v>22977</v>
+        <v>23449</v>
       </c>
       <c r="B224" s="251" t="s">
-        <v>23213</v>
+        <v>23685</v>
       </c>
     </row>
     <row r="225">
       <c r="A225" s="251" t="s">
-        <v>22978</v>
+        <v>23450</v>
       </c>
       <c r="B225" s="251" t="s">
-        <v>23214</v>
+        <v>23686</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" s="251" t="s">
-        <v>22979</v>
+        <v>23451</v>
       </c>
       <c r="B226" s="251" t="s">
-        <v>23215</v>
+        <v>23687</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" s="251" t="s">
-        <v>22980</v>
+        <v>23452</v>
       </c>
       <c r="B227" s="251" t="s">
-        <v>23216</v>
+        <v>23688</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" s="251" t="s">
-        <v>22981</v>
+        <v>23453</v>
       </c>
       <c r="B228" s="251" t="s">
-        <v>23217</v>
+        <v>23689</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" s="251" t="s">
-        <v>22982</v>
+        <v>23454</v>
       </c>
       <c r="B229" s="251" t="s">
-        <v>23218</v>
+        <v>23690</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" s="251" t="s">
-        <v>22983</v>
+        <v>23455</v>
       </c>
       <c r="B230" s="251" t="s">
-        <v>23219</v>
+        <v>23691</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" s="251" t="s">
-        <v>22984</v>
+        <v>23456</v>
       </c>
       <c r="B231" s="251" t="s">
-        <v>23220</v>
+        <v>23692</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" s="251" t="s">
-        <v>22985</v>
+        <v>23457</v>
       </c>
       <c r="B232" s="251" t="s">
-        <v>23221</v>
+        <v>23693</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" s="251" t="s">
-        <v>22986</v>
+        <v>23458</v>
       </c>
       <c r="B233" s="251" t="s">
-        <v>23222</v>
+        <v>23694</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" s="251" t="s">
-        <v>22987</v>
+        <v>23459</v>
       </c>
       <c r="B234" s="251" t="s">
-        <v>23223</v>
+        <v>23695</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" s="251" t="s">
-        <v>22988</v>
+        <v>23460</v>
       </c>
       <c r="B235" s="251" t="s">
-        <v>23224</v>
+        <v>23696</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" s="251" t="s">
-        <v>22989</v>
+        <v>23461</v>
       </c>
       <c r="B236" s="251" t="s">
-        <v>23225</v>
+        <v>23697</v>
       </c>
     </row>
     <row r="237">

</xml_diff>